<commit_message>
[Refactor] format tables for submission
</commit_message>
<xml_diff>
--- a/analysis/Table1-Risk-Factor-Defn.xlsx
+++ b/analysis/Table1-Risk-Factor-Defn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kitty\Documents\Undergrad\COOP\CANHEART\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1335E1C-357C-4C9B-A1C7-96C47449D8A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A75BC8-169E-4912-9049-15C5C60B948B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-4650" windowWidth="29040" windowHeight="15840" xr2:uid="{4A2005D5-DF27-494E-A76B-13E7E83FF1EB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Category</t>
   </si>
@@ -199,12 +199,35 @@
       <t>6 (women) drinks/week</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Table 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Risk factor definitions. Risk health behaviours of interest are marked with (*).</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +245,14 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -285,6 +316,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -295,12 +332,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -617,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E4B917-D697-4085-8427-C6E3A880EF60}">
-  <dimension ref="A2:C22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,6 +661,11 @@
     <col min="3" max="3" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>45</v>
@@ -642,7 +678,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -653,7 +689,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -662,7 +698,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -673,7 +709,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
@@ -682,7 +718,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -693,7 +729,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -702,7 +738,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
@@ -711,7 +747,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
@@ -720,7 +756,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -731,7 +767,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
@@ -740,7 +776,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="4" t="s">
         <v>20</v>
       </c>
@@ -749,7 +785,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -760,7 +796,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
@@ -769,7 +805,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="3" t="s">
         <v>26</v>
       </c>
@@ -778,7 +814,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -789,7 +825,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="2" t="s">
         <v>29</v>
       </c>
@@ -798,7 +834,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="2" t="s">
         <v>30</v>
       </c>
@@ -807,7 +843,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="3" t="s">
         <v>32</v>
       </c>
@@ -816,7 +852,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -827,7 +863,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="5" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
[Refactor] clean up figure data and analysis
Fixed subgroup labelling
</commit_message>
<xml_diff>
--- a/analysis/Table1-Risk-Factor-Defn.xlsx
+++ b/analysis/Table1-Risk-Factor-Defn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kitty\Documents\Undergrad\COOP\CANHEART\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A75BC8-169E-4912-9049-15C5C60B948B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FB9ED5-1186-4047-9C08-13A645A8ECAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4650" windowWidth="29040" windowHeight="15840" xr2:uid="{4A2005D5-DF27-494E-A76B-13E7E83FF1EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4A2005D5-DF27-494E-A76B-13E7E83FF1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>No diabetes</t>
   </si>
   <si>
-    <t>BMI</t>
-  </si>
-  <si>
     <t>BMI ≥ 30</t>
   </si>
   <si>
@@ -87,19 +84,10 @@
     <t>Physical activity</t>
   </si>
   <si>
-    <t>0 to &lt;1.5 METs/day</t>
-  </si>
-  <si>
     <t>Moderately active</t>
   </si>
   <si>
-    <t>1.5 to &lt;3 METs/day</t>
-  </si>
-  <si>
     <t>Active</t>
-  </si>
-  <si>
-    <t>≥ 3 METs/day</t>
   </si>
   <si>
     <t>Smoking</t>
@@ -200,6 +188,18 @@
     </r>
   </si>
   <si>
+    <t>Body Mass Index (BMI)</t>
+  </si>
+  <si>
+    <t>0 to &lt;1.5 MET-hours/day</t>
+  </si>
+  <si>
+    <t>1.5 to &lt;3 MET-hours/day</t>
+  </si>
+  <si>
+    <t>≥ 3 MET-hours/day</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -219,7 +219,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: Risk factor definitions. Risk health behaviours of interest are marked with (*).</t>
+      <t>: Risk factor definitions with categories are marked with (*).</t>
     </r>
   </si>
 </sst>
@@ -306,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -328,11 +328,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -650,7 +656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E4B917-D697-4085-8427-C6E3A880EF60}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -668,7 +674,7 @@
     </row>
     <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -682,7 +688,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -702,7 +708,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -717,158 +723,158 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="C13" s="4" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>